<commit_message>
Flora: Artwerte neu exportiert
</commit_message>
<xml_diff>
--- a/_original/Flora/zh_artwert_1995.xlsx
+++ b/_original/Flora/zh_artwert_1995.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$176</definedName>
     <definedName name="zh_artwert_1995" localSheetId="0">Tabelle1!$A$1:$H$176</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -43,27 +44,6 @@
     <t>GUID</t>
   </si>
   <si>
-    <t>ZH Artwert (1995): Artwert KT ZH</t>
-  </si>
-  <si>
-    <t>ZH Artwert (1995): Artwertberechnung Anteil am CH-Bestand</t>
-  </si>
-  <si>
-    <t>ZH Artwert (1995): Artwertberechnung Areal weltweit</t>
-  </si>
-  <si>
-    <t>ZH Artwert (1995): Artwertberechnung Gefährdung CH Punkte</t>
-  </si>
-  <si>
-    <t>ZH Artwert (1995): Artwertberechnung Gefährdung EU Punkte</t>
-  </si>
-  <si>
-    <t>ZH Artwert (1995): Artwertberechnung Gefährdung ZH Punkte</t>
-  </si>
-  <si>
-    <t>ZH Artwert (1995): Neophyt</t>
-  </si>
-  <si>
     <t>01BD11B2-7B5B-4D5A-95A4-7AF765E7A978</t>
   </si>
   <si>
@@ -611,6 +591,27 @@
   </si>
   <si>
     <t>FAB7F281-8782-4D81-96EA-D2F9858B5960</t>
+  </si>
+  <si>
+    <t>Artwert KT ZH</t>
+  </si>
+  <si>
+    <t>Artwertberechnung Anteil am CH-Bestand</t>
+  </si>
+  <si>
+    <t>Artwertberechnung Areal weltweit</t>
+  </si>
+  <si>
+    <t>Artwertberechnung Gefährdung CH Punkte</t>
+  </si>
+  <si>
+    <t>Artwertberechnung Gefährdung EU Punkte</t>
+  </si>
+  <si>
+    <t>Artwertberechnung Gefährdung ZH Punkte</t>
+  </si>
+  <si>
+    <t>Neophyt</t>
   </si>
 </sst>
 </file>
@@ -956,7 +957,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H176"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -974,532 +977,532 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>184</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>185</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>186</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>187</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>188</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>189</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H2" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H4" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H6" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H8" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H10" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H11" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H12" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H13" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H14" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H15" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H16" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B17">
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H17" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B18">
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H18" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H19" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H20" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H21" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H22" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B23">
         <v>0</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H23" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
       <c r="C24" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H24" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B25">
         <v>0</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H25" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B26">
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H26" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B27">
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H27" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B28">
         <v>0</v>
       </c>
       <c r="C28" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H28" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B29">
         <v>0</v>
       </c>
       <c r="C29" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H29" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B30">
         <v>0</v>
       </c>
       <c r="C30" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H30" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B31">
         <v>0</v>
       </c>
       <c r="C31" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D31" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -1511,395 +1514,395 @@
         <v>0</v>
       </c>
       <c r="H31" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B32">
         <v>0</v>
       </c>
       <c r="C32" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H32" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B33">
         <v>0</v>
       </c>
       <c r="C33" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H33" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B34">
         <v>0</v>
       </c>
       <c r="C34" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H34" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B35">
         <v>7</v>
       </c>
       <c r="C35" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H35" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B36">
         <v>7</v>
       </c>
       <c r="C36" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H36" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B37">
         <v>0</v>
       </c>
       <c r="C37" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H37" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B38">
         <v>0</v>
       </c>
       <c r="C38" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D38" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H38" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B39">
         <v>0</v>
       </c>
       <c r="C39" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D39" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H39" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B40">
         <v>0</v>
       </c>
       <c r="C40" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D40" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H40" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B41">
         <v>0</v>
       </c>
       <c r="C41" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H41" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B42">
         <v>0</v>
       </c>
       <c r="C42" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D42" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H42" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B43">
         <v>0</v>
       </c>
       <c r="C43" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D43" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H43" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B44">
         <v>0</v>
       </c>
       <c r="C44" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D44" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H44" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B45">
         <v>0</v>
       </c>
       <c r="C45" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D45" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H45" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B46">
         <v>0</v>
       </c>
       <c r="C46" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D46" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H46" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B47">
         <v>0</v>
       </c>
       <c r="C47" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D47" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H47" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B48">
         <v>0</v>
       </c>
       <c r="C48" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H48" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B49">
         <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D49" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H49" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B50">
         <v>0</v>
       </c>
       <c r="C50" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D50" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H50" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B51">
         <v>0</v>
       </c>
       <c r="C51" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D51" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H51" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B52">
         <v>3</v>
       </c>
       <c r="C52" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D52" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H52" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B53">
         <v>0</v>
       </c>
       <c r="C53" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H53" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B54">
         <v>8</v>
       </c>
       <c r="C54" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D54" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E54">
         <v>3</v>
@@ -1911,72 +1914,72 @@
         <v>3</v>
       </c>
       <c r="H54" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B55">
         <v>0</v>
       </c>
       <c r="C55" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D55" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H55" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B56">
         <v>0</v>
       </c>
       <c r="C56" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D56" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H56" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B57">
         <v>0</v>
       </c>
       <c r="C57" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D57" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H57" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B58">
         <v>11</v>
       </c>
       <c r="C58" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D58" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E58">
         <v>4</v>
@@ -1988,106 +1991,106 @@
         <v>3</v>
       </c>
       <c r="H58" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B59">
         <v>0</v>
       </c>
       <c r="C59" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D59" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H59" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B60">
         <v>0</v>
       </c>
       <c r="C60" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D60" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H60" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B61">
         <v>0</v>
       </c>
       <c r="C61" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D61" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H61" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B62">
         <v>0</v>
       </c>
       <c r="C62" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D62" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H62" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B63">
         <v>3</v>
       </c>
       <c r="C63" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D63" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H63" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B64">
         <v>12</v>
       </c>
       <c r="C64" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D64" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E64">
         <v>4</v>
@@ -2099,21 +2102,21 @@
         <v>3</v>
       </c>
       <c r="H64" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B65">
         <v>0</v>
       </c>
       <c r="C65" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D65" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E65">
         <v>0</v>
@@ -2125,463 +2128,463 @@
         <v>0</v>
       </c>
       <c r="H65" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B66">
         <v>0</v>
       </c>
       <c r="C66" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D66" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H66" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B67">
         <v>3</v>
       </c>
       <c r="C67" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D67" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H67" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B68">
         <v>0</v>
       </c>
       <c r="C68" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D68" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H68" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B69">
         <v>0</v>
       </c>
       <c r="C69" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D69" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H69" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B70">
         <v>0</v>
       </c>
       <c r="C70" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D70" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H70" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B71">
         <v>2</v>
       </c>
       <c r="C71" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D71" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H71" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B72">
         <v>3</v>
       </c>
       <c r="C72" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D72" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H72" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B73">
         <v>4</v>
       </c>
       <c r="C73" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D73" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H73" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B74">
         <v>0</v>
       </c>
       <c r="C74" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D74" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H74" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B75">
         <v>0</v>
       </c>
       <c r="C75" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D75" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H75" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B76">
         <v>3</v>
       </c>
       <c r="C76" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D76" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H76" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B77">
         <v>0</v>
       </c>
       <c r="C77" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D77" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H77" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B78">
         <v>0</v>
       </c>
       <c r="C78" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D78" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H78" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B79">
         <v>0</v>
       </c>
       <c r="C79" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D79" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H79" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B80">
         <v>0</v>
       </c>
       <c r="C80" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D80" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H80" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B81">
         <v>3</v>
       </c>
       <c r="C81" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D81" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H81" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B82">
         <v>0</v>
       </c>
       <c r="C82" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D82" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H82" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B83">
         <v>0</v>
       </c>
       <c r="C83" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D83" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H83" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B84">
         <v>0</v>
       </c>
       <c r="C84" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D84" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H84" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B85">
         <v>3</v>
       </c>
       <c r="C85" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D85" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H85" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B86">
         <v>0</v>
       </c>
       <c r="C86" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D86" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H86" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B87">
         <v>0</v>
       </c>
       <c r="C87" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D87" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H87" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B88">
         <v>0</v>
       </c>
       <c r="C88" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D88" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H88" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B89">
         <v>4</v>
       </c>
       <c r="C89" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D89" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H89" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B90">
         <v>0</v>
       </c>
       <c r="C90" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D90" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H90" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B91">
         <v>2</v>
       </c>
       <c r="C91" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D91" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H91" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B92">
         <v>0</v>
       </c>
       <c r="C92" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D92" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E92">
         <v>0</v>
@@ -2593,55 +2596,55 @@
         <v>0</v>
       </c>
       <c r="H92" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B93">
         <v>0</v>
       </c>
       <c r="C93" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D93" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H93" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B94">
         <v>0</v>
       </c>
       <c r="C94" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D94" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H94" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B95">
         <v>0</v>
       </c>
       <c r="C95" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D95" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E95">
         <v>0</v>
@@ -2653,38 +2656,38 @@
         <v>0</v>
       </c>
       <c r="H95" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B96">
         <v>0</v>
       </c>
       <c r="C96" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D96" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H96" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B97">
         <v>0</v>
       </c>
       <c r="C97" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D97" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E97">
         <v>0</v>
@@ -2696,732 +2699,732 @@
         <v>0</v>
       </c>
       <c r="H97" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B98">
         <v>4</v>
       </c>
       <c r="C98" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D98" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H98" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B99">
         <v>0</v>
       </c>
       <c r="C99" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D99" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H99" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B100">
         <v>0</v>
       </c>
       <c r="C100" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D100" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H100" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B101">
         <v>3</v>
       </c>
       <c r="C101" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D101" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H101" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B102">
         <v>0</v>
       </c>
       <c r="C102" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D102" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H102" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B103">
         <v>0</v>
       </c>
       <c r="C103" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D103" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H103" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B104">
         <v>3</v>
       </c>
       <c r="C104" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D104" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H104" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B105">
         <v>0</v>
       </c>
       <c r="C105" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D105" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H105" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B106">
         <v>0</v>
       </c>
       <c r="C106" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D106" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H106" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B107">
         <v>0</v>
       </c>
       <c r="C107" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D107" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H107" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B108">
         <v>4</v>
       </c>
       <c r="C108" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D108" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H108" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B109">
         <v>0</v>
       </c>
       <c r="C109" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D109" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H109" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B110">
         <v>0</v>
       </c>
       <c r="C110" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D110" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H110" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B111">
         <v>4</v>
       </c>
       <c r="C111" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D111" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H111" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B112">
         <v>0</v>
       </c>
       <c r="C112" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D112" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H112" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B113">
         <v>2</v>
       </c>
       <c r="C113" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D113" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H113" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B114">
         <v>0</v>
       </c>
       <c r="C114" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D114" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H114" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B115">
         <v>0</v>
       </c>
       <c r="C115" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D115" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H115" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B116">
         <v>5</v>
       </c>
       <c r="C116" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D116" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H116" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B117">
         <v>0</v>
       </c>
       <c r="C117" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D117" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H117" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B118">
         <v>0</v>
       </c>
       <c r="C118" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D118" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H118" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B119">
         <v>3</v>
       </c>
       <c r="C119" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D119" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H119" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B120">
         <v>0</v>
       </c>
       <c r="C120" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D120" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H120" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B121">
         <v>0</v>
       </c>
       <c r="C121" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D121" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H121" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B122">
         <v>0</v>
       </c>
       <c r="C122" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D122" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H122" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B123">
         <v>0</v>
       </c>
       <c r="C123" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D123" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H123" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B124">
         <v>0</v>
       </c>
       <c r="C124" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D124" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H124" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B125">
         <v>0</v>
       </c>
       <c r="C125" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D125" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H125" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B126">
         <v>7</v>
       </c>
       <c r="C126" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D126" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H126" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B127">
         <v>3</v>
       </c>
       <c r="C127" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D127" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H127" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B128">
         <v>0</v>
       </c>
       <c r="C128" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D128" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H128" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B129">
         <v>9</v>
       </c>
       <c r="C129" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D129" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H129" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C130" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D130" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H130" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B131">
         <v>4</v>
       </c>
       <c r="C131" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D131" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H131" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B132">
         <v>0</v>
       </c>
       <c r="C132" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D132" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H132" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B133">
         <v>0</v>
       </c>
       <c r="C133" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D133" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H133" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B134">
         <v>0</v>
       </c>
       <c r="C134" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D134" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H134" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B135">
         <v>0</v>
       </c>
       <c r="C135" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D135" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H135" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B136">
         <v>14</v>
       </c>
       <c r="C136" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D136" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H136" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B137">
         <v>0</v>
       </c>
       <c r="C137" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D137" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H137" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B138">
         <v>0</v>
       </c>
       <c r="C138" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D138" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H138" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B139">
         <v>6</v>
       </c>
       <c r="C139" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D139" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H139" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B140">
         <v>0</v>
       </c>
       <c r="C140" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D140" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E140">
         <v>0</v>
@@ -3433,72 +3436,72 @@
         <v>0</v>
       </c>
       <c r="H140" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B141">
         <v>0</v>
       </c>
       <c r="C141" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D141" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H141" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B142">
         <v>0</v>
       </c>
       <c r="C142" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D142" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H142" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B143">
         <v>0</v>
       </c>
       <c r="C143" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D143" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H143" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B144">
         <v>2</v>
       </c>
       <c r="C144" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D144" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E144">
         <v>0</v>
@@ -3510,157 +3513,157 @@
         <v>0</v>
       </c>
       <c r="H144" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B145">
         <v>0</v>
       </c>
       <c r="C145" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D145" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H145" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B146">
         <v>0</v>
       </c>
       <c r="C146" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D146" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H146" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B147">
         <v>3</v>
       </c>
       <c r="C147" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D147" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H147" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B148">
         <v>0</v>
       </c>
       <c r="C148" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D148" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H148" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B149">
         <v>3</v>
       </c>
       <c r="C149" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D149" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H149" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="B150">
         <v>0</v>
       </c>
       <c r="C150" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D150" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H150" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B151">
         <v>0</v>
       </c>
       <c r="C151" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D151" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H151" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B152">
         <v>0</v>
       </c>
       <c r="C152" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D152" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H152" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B153">
         <v>0</v>
       </c>
       <c r="C153" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D153" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E153">
         <v>0</v>
@@ -3672,327 +3675,327 @@
         <v>0</v>
       </c>
       <c r="H153" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B154">
         <v>0</v>
       </c>
       <c r="C154" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D154" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H154" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B155">
         <v>0</v>
       </c>
       <c r="C155" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D155" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H155" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B156">
         <v>3</v>
       </c>
       <c r="C156" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D156" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H156" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B157">
         <v>0</v>
       </c>
       <c r="C157" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D157" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H157" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B158">
         <v>0</v>
       </c>
       <c r="C158" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D158" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H158" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B159">
         <v>0</v>
       </c>
       <c r="C159" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D159" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H159" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B160">
         <v>0</v>
       </c>
       <c r="C160" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D160" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H160" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B161">
         <v>0</v>
       </c>
       <c r="C161" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D161" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H161" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B162">
         <v>1</v>
       </c>
       <c r="C162" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D162" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H162" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B163">
         <v>0</v>
       </c>
       <c r="C163" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D163" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H163" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="B164">
         <v>0</v>
       </c>
       <c r="C164" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D164" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H164" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="B165">
         <v>0</v>
       </c>
       <c r="C165" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D165" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H165" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="B166">
         <v>0</v>
       </c>
       <c r="C166" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D166" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H166" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="B167">
         <v>0</v>
       </c>
       <c r="C167" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D167" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H167" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B168">
         <v>0</v>
       </c>
       <c r="C168" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D168" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H168" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B169">
         <v>0</v>
       </c>
       <c r="C169" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D169" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H169" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="B170">
         <v>0</v>
       </c>
       <c r="C170" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D170" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H170" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="B171">
         <v>0</v>
       </c>
       <c r="C171" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D171" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H171" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="B172">
         <v>0</v>
       </c>
       <c r="C172" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D172" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E172">
         <v>0</v>
@@ -4004,72 +4007,72 @@
         <v>0</v>
       </c>
       <c r="H172" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B173">
         <v>0</v>
       </c>
       <c r="C173" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D173" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H173" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="B174">
         <v>0</v>
       </c>
       <c r="C174" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D174" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H174" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B175">
         <v>0</v>
       </c>
       <c r="C175" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D175" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H175" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B176">
         <v>0</v>
       </c>
       <c r="C176" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D176" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E176">
         <v>0</v>
@@ -4081,10 +4084,11 @@
         <v>0</v>
       </c>
       <c r="H176" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H176"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>